<commit_message>
CTECH-2652 fix dates as strings (for cut labels)
</commit_message>
<xml_diff>
--- a/examples/features/core-lusid/extracts/holdings_20200105.xlsx
+++ b/examples/features/core-lusid/extracts/holdings_20200105.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,62 +436,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>instrument_uid</t>
+          <t>luid</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sub_holding_keys</t>
+          <t>instrumentName</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Name(default-Properties)</t>
+          <t>holdingType</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>SourcePortfolioId(default-Properties)</t>
+          <t>units</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SourcePortfolioScope(default-Properties)</t>
+          <t>settledUnits</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>holding_type</t>
+          <t>costAmount</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>units</t>
+          <t>costCurrency</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>settled_units</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>cost.amount</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>cost.currency</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>cost_portfolio_ccy.amount</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>cost_portfolio_ccy.currency</t>
+          <t>portfolioCurrency</t>
         </is>
       </c>
     </row>
@@ -439,47 +486,29 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Aviva</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Aviva</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="E2" t="n">
         <v>132000</v>
       </c>
-      <c r="I2" t="n">
+      <c r="F2" t="n">
         <v>132000</v>
       </c>
-      <c r="J2" t="n">
+      <c r="G2" t="n">
         <v>660000</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -496,47 +525,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>BHP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BHP</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="E3" t="n">
         <v>120000</v>
       </c>
-      <c r="I3" t="n">
+      <c r="F3" t="n">
         <v>120000</v>
       </c>
-      <c r="J3" t="n">
+      <c r="G3" t="n">
         <v>2160000</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -553,47 +564,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Barclays</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Barclays</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="E4" t="n">
         <v>300000</v>
       </c>
-      <c r="I4" t="n">
+      <c r="F4" t="n">
         <v>300000</v>
       </c>
-      <c r="J4" t="n">
+      <c r="G4" t="n">
         <v>600000</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -610,47 +603,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BP</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="E5" t="n">
         <v>200000</v>
       </c>
-      <c r="I5" t="n">
+      <c r="F5" t="n">
         <v>200000</v>
       </c>
-      <c r="J5" t="n">
+      <c r="G5" t="n">
         <v>1000000</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -667,47 +642,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>HSBC</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HSBC</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="E6" t="n">
         <v>40000</v>
       </c>
-      <c r="I6" t="n">
+      <c r="F6" t="n">
         <v>40000</v>
       </c>
-      <c r="J6" t="n">
+      <c r="G6" t="n">
         <v>240000</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="inlineStr">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -724,53 +681,35 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CCY_GBP</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="E7" t="n">
         <v>7340000</v>
       </c>
-      <c r="I7" t="n">
+      <c r="F7" t="n">
         <v>7340000</v>
       </c>
-      <c r="J7" t="n">
+      <c r="G7" t="n">
         <v>7340000</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="inlineStr">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CTECH-2652 fix dates as strings (for cut labels) (#611)
</commit_message>
<xml_diff>
--- a/examples/features/core-lusid/extracts/holdings_20200105.xlsx
+++ b/examples/features/core-lusid/extracts/holdings_20200105.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,62 +436,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>instrument_uid</t>
+          <t>luid</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sub_holding_keys</t>
+          <t>instrumentName</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Name(default-Properties)</t>
+          <t>holdingType</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>SourcePortfolioId(default-Properties)</t>
+          <t>units</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SourcePortfolioScope(default-Properties)</t>
+          <t>settledUnits</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>holding_type</t>
+          <t>costAmount</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>units</t>
+          <t>costCurrency</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>settled_units</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>cost.amount</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>cost.currency</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>cost_portfolio_ccy.amount</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>cost_portfolio_ccy.currency</t>
+          <t>portfolioCurrency</t>
         </is>
       </c>
     </row>
@@ -439,47 +486,29 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Aviva</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Aviva</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="E2" t="n">
         <v>132000</v>
       </c>
-      <c r="I2" t="n">
+      <c r="F2" t="n">
         <v>132000</v>
       </c>
-      <c r="J2" t="n">
+      <c r="G2" t="n">
         <v>660000</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -496,47 +525,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>BHP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BHP</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="E3" t="n">
         <v>120000</v>
       </c>
-      <c r="I3" t="n">
+      <c r="F3" t="n">
         <v>120000</v>
       </c>
-      <c r="J3" t="n">
+      <c r="G3" t="n">
         <v>2160000</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -553,47 +564,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Barclays</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Barclays</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="E4" t="n">
         <v>300000</v>
       </c>
-      <c r="I4" t="n">
+      <c r="F4" t="n">
         <v>300000</v>
       </c>
-      <c r="J4" t="n">
+      <c r="G4" t="n">
         <v>600000</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -610,47 +603,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BP</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="E5" t="n">
         <v>200000</v>
       </c>
-      <c r="I5" t="n">
+      <c r="F5" t="n">
         <v>200000</v>
       </c>
-      <c r="J5" t="n">
+      <c r="G5" t="n">
         <v>1000000</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -667,47 +642,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>HSBC</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HSBC</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="E6" t="n">
         <v>40000</v>
       </c>
-      <c r="I6" t="n">
+      <c r="F6" t="n">
         <v>40000</v>
       </c>
-      <c r="J6" t="n">
+      <c r="G6" t="n">
         <v>240000</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="inlineStr">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -724,53 +681,35 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CCY_GBP</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>EQUITY_UK</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3892-f315-6c98-9a</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
           <t>B</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="E7" t="n">
         <v>7340000</v>
       </c>
-      <c r="I7" t="n">
+      <c r="F7" t="n">
         <v>7340000</v>
       </c>
-      <c r="J7" t="n">
+      <c r="G7" t="n">
         <v>7340000</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="inlineStr">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>